<commit_message>
functionality, session streamlined and styling
</commit_message>
<xml_diff>
--- a/Documentatie/Taakverdeling.xlsx
+++ b/Documentatie/Taakverdeling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Baqme\Baqme-examen\Baqme-examen\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71C580D-9652-4668-93FE-6DF99617EB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BC04D4-CC38-4C1F-B09B-3D0FF3C09181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A4BEF21F-CE1A-4BCD-ACA2-1CDEE795526A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Datum</t>
   </si>
@@ -90,6 +90,30 @@
   </si>
   <si>
     <t>Animations met CSS &amp; JS</t>
+  </si>
+  <si>
+    <t>Account update &amp; delete geimplementeerd</t>
+  </si>
+  <si>
+    <t>Account registratie pagina gemaakt de en functionaliteit hiervan gemaakt</t>
+  </si>
+  <si>
+    <t>Styling van het dashboard opnieuw bedacht en gemaakt</t>
+  </si>
+  <si>
+    <t>Verder gewerkt aan de navbar, want er waren meerdere problemen mee</t>
+  </si>
+  <si>
+    <t>Layout van de dashboard pagina opnieuw bedacht (ivm feedback stagebegeleider)</t>
+  </si>
+  <si>
+    <t>Login en registratie-pagina's afgemaakt</t>
+  </si>
+  <si>
+    <t>Database gegevens weergeven in de submenu van de navbar</t>
+  </si>
+  <si>
+    <t>Functionaliteiten van de account management aangepast zodat alleen admin accounts hier bij kunnen</t>
   </si>
 </sst>
 </file>
@@ -137,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -160,11 +184,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -177,6 +214,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -511,14 +552,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4B3641-1EB0-4538-8AA3-F29F92B43BAB}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -694,14 +736,126 @@
       <c r="A13" s="7">
         <v>45539</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="8">
         <v>120</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45569</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3">
+        <v>240</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45569</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3">
+        <v>180</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45600</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="5">
+        <v>360</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45600</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="5">
+        <v>80</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45600</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3">
+        <v>80</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45600</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3">
+        <v>120</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45600</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3">
+        <v>80</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>45600</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3">
+        <v>80</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>